<commit_message>
Working on mass and charge balance
</commit_message>
<xml_diff>
--- a/python/multiscalepy/multiscale/modelcreator/models/demo/demo_annotations.xlsx
+++ b/python/multiscalepy/multiscale/modelcreator/models/demo/demo_annotations.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="68">
   <si>
     <t>pattern</t>
   </si>
@@ -180,6 +180,21 @@
   </si>
   <si>
     <t>^\w{1}__C$</t>
+  </si>
+  <si>
+    <t>^\w{1}__\w+$</t>
+  </si>
+  <si>
+    <t>Formula</t>
+  </si>
+  <si>
+    <t>C6H12O6</t>
+  </si>
+  <si>
+    <t>Charge</t>
+  </si>
+  <si>
+    <t>0</t>
   </si>
   <si>
     <t># reactions</t>
@@ -219,6 +234,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -236,12 +252,6 @@
       <family val="0"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
       <b val="true"/>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -255,6 +265,13 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="5">
@@ -317,56 +334,60 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -374,7 +395,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -459,10 +480,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G31"/>
+  <dimension ref="A1:G32"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D33" activeCellId="0" sqref="D33"/>
+      <selection pane="topLeft" activeCell="D29" activeCellId="0" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -550,6 +571,15 @@
         <v>18</v>
       </c>
     </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0"/>
+      <c r="B5" s="0"/>
+      <c r="C5" s="0"/>
+      <c r="D5" s="0"/>
+      <c r="E5" s="0"/>
+      <c r="F5" s="0"/>
+      <c r="G5" s="0"/>
+    </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="4" t="s">
         <v>19</v>
@@ -787,8 +817,13 @@
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0"/>
+      <c r="B18" s="0"/>
+      <c r="C18" s="0"/>
       <c r="D18" s="10"/>
+      <c r="E18" s="0"/>
       <c r="F18" s="9"/>
+      <c r="G18" s="0"/>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="4" t="s">
@@ -870,6 +905,15 @@
         <v>47</v>
       </c>
     </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="0"/>
+      <c r="B23" s="0"/>
+      <c r="C23" s="0"/>
+      <c r="D23" s="0"/>
+      <c r="E23" s="0"/>
+      <c r="F23" s="0"/>
+      <c r="G23" s="0"/>
+    </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="4" t="s">
         <v>48</v>
@@ -951,55 +995,62 @@
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D28" s="10"/>
+      <c r="A28" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="B28" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="C28" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="D28" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="E28" s="0"/>
       <c r="F28" s="9"/>
+      <c r="G28" s="0"/>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="4" t="s">
+      <c r="A29" s="16" t="s">
         <v>55</v>
       </c>
-      <c r="B29" s="5"/>
-      <c r="C29" s="5"/>
-      <c r="D29" s="6"/>
-      <c r="E29" s="5"/>
-      <c r="F29" s="5"/>
-      <c r="G29" s="5"/>
-    </row>
-    <row r="30" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="B30" s="9" t="s">
-        <v>57</v>
-      </c>
-      <c r="C30" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="D30" s="11" t="s">
+      <c r="B29" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="C29" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="E30" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="F30" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="G30" s="15" t="s">
+      <c r="D29" s="10" t="s">
         <v>59</v>
       </c>
+      <c r="E29" s="9"/>
+      <c r="F29" s="9"/>
+      <c r="G29" s="0"/>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="B30" s="5"/>
+      <c r="C30" s="5"/>
+      <c r="D30" s="6"/>
+      <c r="E30" s="5"/>
+      <c r="F30" s="5"/>
+      <c r="G30" s="5"/>
     </row>
     <row r="31" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="7" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B31" s="9" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
       <c r="C31" s="9" t="s">
         <v>9</v>
       </c>
       <c r="D31" s="11" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="E31" s="9" t="s">
         <v>23</v>
@@ -1008,7 +1059,30 @@
         <v>12</v>
       </c>
       <c r="G31" s="15" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="B32" s="9" t="s">
         <v>62</v>
+      </c>
+      <c r="C32" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="D32" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="E32" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="F32" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="G32" s="15" t="s">
+        <v>67</v>
       </c>
     </row>
   </sheetData>

</xml_diff>